<commit_message>
Ajout temps différents seuils rapport
</commit_message>
<xml_diff>
--- a/tp1/z-ancienRawCorrect/mean/strassSeuilAncien.xlsx
+++ b/tp1/z-ancienRawCorrect/mean/strassSeuilAncien.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C6BAB13-E3F8-4A5D-BC28-3173A3302BB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7C374707-0103-42BA-A636-5D0E6039537B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71:F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1544,7 +1544,7 @@
         <v>9.9430084228515508E-4</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:G59" si="4">AVERAGE(C42:C51)</f>
+        <f t="shared" ref="C57:G57" si="4">AVERAGE(C42:C51)</f>
         <v>1.1814928054809545E-2</v>
       </c>
       <c r="D57">
@@ -1714,6 +1714,240 @@
         <v>56.435250997543278</v>
       </c>
     </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>32</v>
+      </c>
+      <c r="B65">
+        <v>9.9430084228515508E-4</v>
+      </c>
+      <c r="C65">
+        <v>1.1814928054809545E-2</v>
+      </c>
+      <c r="D65">
+        <v>0.10464911460876436</v>
+      </c>
+      <c r="E65">
+        <v>1.0316311359405494</v>
+      </c>
+      <c r="F65">
+        <v>6.2837499618530224</v>
+      </c>
+      <c r="G65">
+        <v>57.158779430389359</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>1.221466064453123E-3</v>
+      </c>
+      <c r="C66">
+        <v>1.7058372497558549E-2</v>
+      </c>
+      <c r="D66">
+        <v>0.11063396930694544</v>
+      </c>
+      <c r="E66">
+        <v>0.83319253921508718</v>
+      </c>
+      <c r="F66">
+        <v>6.0393702268600418</v>
+      </c>
+      <c r="G66">
+        <v>49.988905930519067</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>128</v>
+      </c>
+      <c r="B67">
+        <v>2.8555870056152319E-3</v>
+      </c>
+      <c r="C67">
+        <v>2.012114524841303E-2</v>
+      </c>
+      <c r="D67">
+        <v>0.18633048534393248</v>
+      </c>
+      <c r="E67">
+        <v>0.93693289756774834</v>
+      </c>
+      <c r="F67">
+        <v>6.4785861730575505</v>
+      </c>
+      <c r="G67">
+        <v>45.12782776355742</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>256</v>
+      </c>
+      <c r="B68">
+        <v>1.3973236083984349E-3</v>
+      </c>
+      <c r="C68">
+        <v>1.06720685958862E-2</v>
+      </c>
+      <c r="D68">
+        <v>0.11173708438873257</v>
+      </c>
+      <c r="E68">
+        <v>0.87236082553863381</v>
+      </c>
+      <c r="F68">
+        <v>5.6250489950179992</v>
+      </c>
+      <c r="G68">
+        <v>41.073178339004471</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>512</v>
+      </c>
+      <c r="B69">
+        <v>2.1373033523559549E-3</v>
+      </c>
+      <c r="C69">
+        <v>1.489279270172115E-2</v>
+      </c>
+      <c r="D69">
+        <v>0.10714466571807808</v>
+      </c>
+      <c r="E69">
+        <v>0.86393249034881558</v>
+      </c>
+      <c r="F69">
+        <v>6.7058665513992253</v>
+      </c>
+      <c r="G69">
+        <v>56.435250997543278</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70">
+        <v>32</v>
+      </c>
+      <c r="C70">
+        <v>64</v>
+      </c>
+      <c r="D70">
+        <v>128</v>
+      </c>
+      <c r="E70">
+        <v>256</v>
+      </c>
+      <c r="F70">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71">
+        <v>9.9430084228515508E-4</v>
+      </c>
+      <c r="C71">
+        <v>1.221466064453123E-3</v>
+      </c>
+      <c r="D71">
+        <v>2.8555870056152319E-3</v>
+      </c>
+      <c r="E71">
+        <v>1.3973236083984349E-3</v>
+      </c>
+      <c r="F71">
+        <v>2.1373033523559549E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72">
+        <v>1.1814928054809545E-2</v>
+      </c>
+      <c r="C72">
+        <v>1.7058372497558549E-2</v>
+      </c>
+      <c r="D72">
+        <v>2.012114524841303E-2</v>
+      </c>
+      <c r="E72">
+        <v>1.06720685958862E-2</v>
+      </c>
+      <c r="F72">
+        <v>1.489279270172115E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73">
+        <v>0.10464911460876436</v>
+      </c>
+      <c r="C73">
+        <v>0.11063396930694544</v>
+      </c>
+      <c r="D73">
+        <v>0.18633048534393248</v>
+      </c>
+      <c r="E73">
+        <v>0.11173708438873257</v>
+      </c>
+      <c r="F73">
+        <v>0.10714466571807808</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74">
+        <v>1.0316311359405494</v>
+      </c>
+      <c r="C74">
+        <v>0.83319253921508718</v>
+      </c>
+      <c r="D74">
+        <v>0.93693289756774834</v>
+      </c>
+      <c r="E74">
+        <v>0.87236082553863381</v>
+      </c>
+      <c r="F74">
+        <v>0.86393249034881558</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B75">
+        <v>6.2837499618530224</v>
+      </c>
+      <c r="C75">
+        <v>6.0393702268600418</v>
+      </c>
+      <c r="D75">
+        <v>6.4785861730575505</v>
+      </c>
+      <c r="E75">
+        <v>5.6250489950179992</v>
+      </c>
+      <c r="F75">
+        <v>6.7058665513992253</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B76">
+        <v>57.158779430389359</v>
+      </c>
+      <c r="C76">
+        <v>49.988905930519067</v>
+      </c>
+      <c r="D76">
+        <v>45.12782776355742</v>
+      </c>
+      <c r="E76">
+        <v>41.073178339004471</v>
+      </c>
+      <c r="F76">
+        <v>56.435250997543278</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>